<commit_message>
checked and changed some names - tnguyen
git-svn-id: svn+ssh://localhost/home/pcb/svn@573 265e18a8-33ca-405d-8757-c40a9e3cabe4
</commit_message>
<xml_diff>
--- a/Bill of Materials masterlist/External/Case/Bill of Materials - Case.xlsx
+++ b/Bill of Materials masterlist/External/Case/Bill of Materials - Case.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Case</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Solar Panel Plates</t>
   </si>
   <si>
-    <t>Baseplate</t>
-  </si>
-  <si>
     <t>Receiver Housing</t>
   </si>
   <si>
@@ -91,6 +88,21 @@
   </si>
   <si>
     <t>Procurement Cost</t>
+  </si>
+  <si>
+    <t>Tray 0</t>
+  </si>
+  <si>
+    <t>Made by</t>
+  </si>
+  <si>
+    <t>S. Bartlett</t>
+  </si>
+  <si>
+    <t>Edited by</t>
+  </si>
+  <si>
+    <t>T. Nguyen</t>
   </si>
 </sst>
 </file>
@@ -449,22 +461,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -482,22 +494,22 @@
         <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -661,7 +673,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -683,9 +695,9 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="F12">
         <v>2</v>
       </c>
       <c r="H12">
@@ -705,9 +717,9 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="B13">
         <v>2</v>
       </c>
       <c r="H13">
@@ -727,7 +739,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14">
         <f>B14+C14+D14+E14+F14+G14</f>
@@ -738,15 +750,15 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" t="s">
         <v>13</v>
-      </c>
-      <c r="M14" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15">
         <v>8</v>
@@ -766,7 +778,23 @@
         <v>2</v>
       </c>
       <c r="M15" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>